<commit_message>
march 1 2020 update
</commit_message>
<xml_diff>
--- a/Master lists/PREPRINTS/PREPRINT_DOIMETADATA_MASTER.xlsx
+++ b/Master lists/PREPRINTS/PREPRINT_DOIMETADATA_MASTER.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ISO_Common\WERB\NIST Publication Series\Crossref Metadata\TechPubs2HTML\Master lists\PREPRINTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE029A1D-68DD-4268-A82D-F687B9BC0251}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FADDF145-B151-4560-87D7-023AEE05CD46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="210">
   <si>
     <t>DOI Created</t>
   </si>
@@ -58,9 +58,6 @@
     <t>2018-09-19T20:20:59Z</t>
   </si>
   <si>
-    <t>IR</t>
-  </si>
-  <si>
     <t>NIST Scientific Foundation Reviews</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>2018-10-31T13:29:47Z</t>
   </si>
   <si>
-    <t>SP</t>
-  </si>
-  <si>
     <t>Proposed Standard Terminology for Robotic Hands and Associated Performance Metrics</t>
   </si>
   <si>
@@ -340,9 +334,6 @@
     <t>2019-09-25T10:14:36Z</t>
   </si>
   <si>
-    <t>CSWP</t>
-  </si>
-  <si>
     <t>A Taxonomic Approach to Understanding Emerging Blockchain Identity Management Systems</t>
   </si>
   <si>
@@ -424,7 +415,7 @@
     <t xml:space="preserve">   2019-10-30T14:32:40Z</t>
   </si>
   <si>
-    <t>2019-10-30T14:32:41Z</t>
+    <t>2019-12-31T19:19:26Z</t>
   </si>
   <si>
     <t>A taxonomy and terminology of adversarial machine learning</t>
@@ -478,7 +469,7 @@
     <t xml:space="preserve">   2019-11-20T14:07:59Z</t>
   </si>
   <si>
-    <t>2019-11-20T14:07:59Z</t>
+    <t>2019-12-31T19:19:28Z</t>
   </si>
   <si>
     <t>Automation Support for Security Control Assessments: Software Vulnerability Management</t>
@@ -529,7 +520,7 @@
     <t>https://nvlpubs.nist.gov/nistpubs/SpecialPublications/NIST.SP.800-189-draft2.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">      2020-01-06T20:27:04Z</t>
+    <t xml:space="preserve">   2020-01-06T20:27:04Z</t>
   </si>
   <si>
     <t>2020-01-07T14:07:05Z</t>
@@ -542,6 +533,123 @@
   </si>
   <si>
     <t>https://nvlpubs.nist.gov/nistpubs/ir/2020/NIST.IR.8259-draft2.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-01-21T19:30:36Z</t>
+  </si>
+  <si>
+    <t>2020-01-22T12:36:57Z</t>
+  </si>
+  <si>
+    <t>Security and Privacy Controls for Information Systems and Organizations</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.SP.800-53r5-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/SpecialPublications/NIST.SP.800-53r5-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-01-24T20:49:59Z</t>
+  </si>
+  <si>
+    <t>2020-01-31T15:35:16Z</t>
+  </si>
+  <si>
+    <t>National Cybersecurity Online Informative References (OLIR) Program:Guidance for OLIR Users and Developers</t>
+  </si>
+  <si>
+    <t>Keller, Nicole; Quinn, Stephen; Scarfone, Karen; Smith, Matthew; Johnson, Vincent</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.IR.8278-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/ir/2020/NIST.IR.8278-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-01-17T18:47:16Z</t>
+  </si>
+  <si>
+    <t>2020-01-17T18:47:18Z</t>
+  </si>
+  <si>
+    <t>Building Secure Microservices-based Applications Using Service-Mesh Architecture</t>
+  </si>
+  <si>
+    <t>Chandramouli, Ramaswamy; Butcher, Zack</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.SP.800-204A-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/SpecialPublications/NIST.SP.800-204A-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-01-13T14:34:35Z</t>
+  </si>
+  <si>
+    <t>2020-01-13T14:34:35Z</t>
+  </si>
+  <si>
+    <t>Assessing Information Security Continuous Monitoring (ISCM) Programs:Developing an ISCM Program Assessment</t>
+  </si>
+  <si>
+    <t>Dempsey, Kelley; Pillitteri, Victoria Yan; Baer, Chad; Niemeyer, Robert; Rudman, Ron; Urban, Susan</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.SP.800-137A-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/SpecialPublications/NIST.SP.800-137A-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-02-03T15:28:49Z</t>
+  </si>
+  <si>
+    <t>2020-02-03T15:28:49Z</t>
+  </si>
+  <si>
+    <t>Key Practices in Cyber Supply Chain Risk Management: Observations from Industry</t>
+  </si>
+  <si>
+    <t>Boyens, Jon M.</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.IR.8276-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/ir/2020/NIST.IR.8276-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-02-10T14:20:00Z</t>
+  </si>
+  <si>
+    <t>2020-02-10T14:20:00Z</t>
+  </si>
+  <si>
+    <t>National Vulnerability Database (NVD) Metadata Submission Guidelines for Common Vulnerabilities and Exposures (CVE) Numbering Authorities (CNAs) and Authorized Data Publishers</t>
+  </si>
+  <si>
+    <t>Byers, Robert; Waltermire, David; Turner, Christopher</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.IR.8246-draft</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/ir/2020/NIST.IR.8246-draft.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   2020-02-13T13:53:43Z</t>
+  </si>
+  <si>
+    <t>2020-02-13T13:53:56Z</t>
+  </si>
+  <si>
+    <t>10.6028/NIST.SP.800-207-draft2</t>
+  </si>
+  <si>
+    <t>https://nvlpubs.nist.gov/nistpubs/SpecialPublications/NIST.SP.800-207-draft2.pdf</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1490,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1427,9 +1535,6 @@
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
       <c r="E2">
         <v>2018</v>
       </c>
@@ -1437,27 +1542,24 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>2018</v>
@@ -1466,27 +1568,24 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
         <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
       </c>
       <c r="E4">
         <v>2018</v>
@@ -1495,27 +1594,24 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>2018</v>
@@ -1524,27 +1620,24 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>2018</v>
@@ -1553,27 +1646,24 @@
         <v>11</v>
       </c>
       <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E7">
         <v>2018</v>
@@ -1582,27 +1672,24 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
         <v>42</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>43</v>
-      </c>
-      <c r="I7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>2019</v>
@@ -1611,27 +1698,24 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>49</v>
-      </c>
-      <c r="I8" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>2019</v>
@@ -1640,27 +1724,24 @@
         <v>2</v>
       </c>
       <c r="G9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>55</v>
-      </c>
-      <c r="I9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="E10">
         <v>2019</v>
@@ -1669,27 +1750,24 @@
         <v>3</v>
       </c>
       <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" t="s">
         <v>60</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>61</v>
-      </c>
-      <c r="I10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>2019</v>
@@ -1698,27 +1776,24 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" t="s">
         <v>66</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>67</v>
-      </c>
-      <c r="I11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="E12">
         <v>2018</v>
@@ -1727,24 +1802,21 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
         <v>72</v>
-      </c>
-      <c r="I12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E13">
         <v>2019</v>
@@ -1753,27 +1825,24 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
         <v>77</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>78</v>
-      </c>
-      <c r="I13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="E14">
         <v>2019</v>
@@ -1782,27 +1851,24 @@
         <v>5</v>
       </c>
       <c r="G14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s">
         <v>82</v>
-      </c>
-      <c r="H14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" t="s">
-        <v>83</v>
-      </c>
-      <c r="J14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="E15">
         <v>2019</v>
@@ -1811,27 +1877,24 @@
         <v>5</v>
       </c>
       <c r="G15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" t="s">
         <v>86</v>
-      </c>
-      <c r="H15" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="E16">
         <v>2019</v>
@@ -1840,24 +1903,21 @@
         <v>4</v>
       </c>
       <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" t="s">
         <v>91</v>
-      </c>
-      <c r="I16" t="s">
-        <v>92</v>
-      </c>
-      <c r="J16" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="E17">
         <v>2019</v>
@@ -1866,24 +1926,21 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" t="s">
         <v>96</v>
-      </c>
-      <c r="I17" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="E18">
         <v>2019</v>
@@ -1892,24 +1949,21 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" t="s">
         <v>101</v>
-      </c>
-      <c r="I18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E19">
         <v>2019</v>
@@ -1918,24 +1972,21 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="E20">
         <v>2019</v>
@@ -1944,27 +1995,24 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" t="s">
+        <v>111</v>
+      </c>
+      <c r="J20" t="s">
         <v>112</v>
-      </c>
-      <c r="H20" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" t="s">
-        <v>114</v>
-      </c>
-      <c r="J20" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="E21">
         <v>2019</v>
@@ -1973,27 +2021,24 @@
         <v>9</v>
       </c>
       <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" t="s">
+        <v>116</v>
+      </c>
+      <c r="I21" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" t="s">
         <v>118</v>
-      </c>
-      <c r="H21" t="s">
-        <v>119</v>
-      </c>
-      <c r="I21" t="s">
-        <v>120</v>
-      </c>
-      <c r="J21" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="E22">
         <v>2019</v>
@@ -2002,27 +2047,24 @@
         <v>10</v>
       </c>
       <c r="G22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
         <v>124</v>
-      </c>
-      <c r="H22" t="s">
-        <v>125</v>
-      </c>
-      <c r="I22" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
-      </c>
-      <c r="C23" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="E23">
         <v>2019</v>
@@ -2031,27 +2073,24 @@
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
+        <v>131</v>
       </c>
       <c r="E24">
         <v>2019</v>
@@ -2060,27 +2099,24 @@
         <v>10</v>
       </c>
       <c r="G24" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" t="s">
+        <v>133</v>
+      </c>
+      <c r="I24" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" t="s">
         <v>135</v>
-      </c>
-      <c r="H24" t="s">
-        <v>136</v>
-      </c>
-      <c r="I24" t="s">
-        <v>137</v>
-      </c>
-      <c r="J24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="E25">
         <v>2019</v>
@@ -2089,27 +2125,24 @@
         <v>10</v>
       </c>
       <c r="G25" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" t="s">
+        <v>139</v>
+      </c>
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25" t="s">
         <v>141</v>
-      </c>
-      <c r="H25" t="s">
-        <v>142</v>
-      </c>
-      <c r="I25" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E26">
         <v>2018</v>
@@ -2118,27 +2151,24 @@
         <v>12</v>
       </c>
       <c r="G26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" t="s">
         <v>42</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>43</v>
-      </c>
-      <c r="I26" t="s">
-        <v>44</v>
-      </c>
-      <c r="J26" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="E27">
         <v>2019</v>
@@ -2147,27 +2177,24 @@
         <v>11</v>
       </c>
       <c r="G27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" t="s">
+        <v>146</v>
+      </c>
+      <c r="J27" t="s">
         <v>147</v>
-      </c>
-      <c r="H27" t="s">
-        <v>148</v>
-      </c>
-      <c r="I27" t="s">
-        <v>149</v>
-      </c>
-      <c r="J27" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
+        <v>149</v>
       </c>
       <c r="E28">
         <v>2019</v>
@@ -2176,27 +2203,24 @@
         <v>11</v>
       </c>
       <c r="G28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" t="s">
         <v>153</v>
-      </c>
-      <c r="H28" t="s">
-        <v>154</v>
-      </c>
-      <c r="I28" t="s">
-        <v>155</v>
-      </c>
-      <c r="J28" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" t="s">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="E29">
         <v>2019</v>
@@ -2205,27 +2229,24 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
+        <v>156</v>
+      </c>
+      <c r="H29" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" t="s">
+        <v>158</v>
+      </c>
+      <c r="J29" t="s">
         <v>159</v>
-      </c>
-      <c r="H29" t="s">
-        <v>160</v>
-      </c>
-      <c r="I29" t="s">
-        <v>161</v>
-      </c>
-      <c r="J29" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E30">
         <v>2019</v>
@@ -2234,27 +2255,24 @@
         <v>5</v>
       </c>
       <c r="G30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I30" t="s">
         <v>77</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>78</v>
-      </c>
-      <c r="I30" t="s">
-        <v>79</v>
-      </c>
-      <c r="J30" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="E31">
         <v>2019</v>
@@ -2263,27 +2281,24 @@
         <v>5</v>
       </c>
       <c r="G31" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" t="s">
+        <v>81</v>
+      </c>
+      <c r="J31" t="s">
         <v>82</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="E32">
         <v>2019</v>
@@ -2292,27 +2307,24 @@
         <v>5</v>
       </c>
       <c r="G32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" t="s">
+        <v>85</v>
+      </c>
+      <c r="J32" t="s">
         <v>86</v>
-      </c>
-      <c r="H32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" t="s">
-        <v>87</v>
-      </c>
-      <c r="J32" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
-      </c>
-      <c r="C33" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="E33">
         <v>2019</v>
@@ -2321,27 +2333,24 @@
         <v>10</v>
       </c>
       <c r="G33" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" t="s">
+        <v>164</v>
+      </c>
+      <c r="J33" t="s">
         <v>165</v>
-      </c>
-      <c r="H33" t="s">
-        <v>166</v>
-      </c>
-      <c r="I33" t="s">
-        <v>167</v>
-      </c>
-      <c r="J33" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
       <c r="E34">
         <v>2020</v>
@@ -2350,16 +2359,195 @@
         <v>1</v>
       </c>
       <c r="G34" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" t="s">
+        <v>169</v>
+      </c>
+      <c r="J34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>171</v>
       </c>
-      <c r="H34" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="B35" t="s">
         <v>172</v>
       </c>
-      <c r="J34" t="s">
+      <c r="E35">
+        <v>2020</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>173</v>
+      </c>
+      <c r="I35" t="s">
+        <v>174</v>
+      </c>
+      <c r="J35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>176</v>
+      </c>
+      <c r="B36" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36">
+        <v>2020</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>178</v>
+      </c>
+      <c r="H36" t="s">
+        <v>179</v>
+      </c>
+      <c r="I36" t="s">
+        <v>180</v>
+      </c>
+      <c r="J36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37">
+        <v>2020</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>184</v>
+      </c>
+      <c r="H37" t="s">
+        <v>185</v>
+      </c>
+      <c r="I37" t="s">
+        <v>186</v>
+      </c>
+      <c r="J37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="E38">
+        <v>2020</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>190</v>
+      </c>
+      <c r="H38" t="s">
+        <v>191</v>
+      </c>
+      <c r="I38" t="s">
+        <v>192</v>
+      </c>
+      <c r="J38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39">
+        <v>2020</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>196</v>
+      </c>
+      <c r="H39" t="s">
+        <v>197</v>
+      </c>
+      <c r="I39" t="s">
+        <v>198</v>
+      </c>
+      <c r="J39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" t="s">
+        <v>201</v>
+      </c>
+      <c r="E40">
+        <v>2020</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>202</v>
+      </c>
+      <c r="H40" t="s">
+        <v>203</v>
+      </c>
+      <c r="I40" t="s">
+        <v>204</v>
+      </c>
+      <c r="J40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E41">
+        <v>2020</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I41" t="s">
+        <v>208</v>
+      </c>
+      <c r="J41" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>